<commit_message>
added purging of channel before stream
</commit_message>
<xml_diff>
--- a/test_files/test_schedule_1_mock_good.xlsx
+++ b/test_files/test_schedule_1_mock_good.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.mitter\Documents\streamscheduler\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35315958-4C74-4FFC-BB3C-6CBC8C940F9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF91A8-6F98-4315-B736-1DFF74E05CDC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_schedule_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>test_files/vids/test4.mp4</t>
+  </si>
+  <si>
+    <t>API_KEY</t>
+  </si>
+  <si>
+    <t>CHANNEL_ID</t>
   </si>
 </sst>
 </file>
@@ -912,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,19 +979,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="46.26953125" customWidth="1"/>
     <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -998,8 +1005,14 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12345</v>
       </c>
@@ -1011,6 +1024,12 @@
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="E2">
+        <v>12345</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>